<commit_message>
Add some Alura content
</commit_message>
<xml_diff>
--- a/business/excel I/Relatório_Cursos.xlsx
+++ b/business/excel I/Relatório_Cursos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>ALUNO</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Café</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>PRODUTO</t>
   </si>
   <si>
@@ -136,6 +133,21 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Total (SUM)</t>
+  </si>
+  <si>
+    <t>Qtd dos Tipos de Itens Vendidos (COUNT.NUM)</t>
+  </si>
+  <si>
+    <t>Qtd dos Tipos de Itens (COUNT.VALORES)</t>
+  </si>
+  <si>
+    <t>Qtd dos Tipos de Itens Não Vendidos (CONTAR.VAZIO)</t>
+  </si>
+  <si>
+    <t>MÉDIA</t>
   </si>
 </sst>
 </file>
@@ -146,7 +158,7 @@
     <numFmt numFmtId="164" formatCode="_-[$R$-416]* #,##0.00_-;\-[$R$-416]* #,##0.00_-;_-[$R$-416]* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +211,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -221,7 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,6 +279,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -795,7 +815,7 @@
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="57.7109375" customWidth="1"/>
     <col min="5" max="5" width="26.85546875" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" customWidth="1"/>
@@ -803,7 +823,7 @@
   <sheetData>
     <row r="3" spans="1:8">
       <c r="B3" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -811,19 +831,19 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -878,10 +898,7 @@
       <c r="D8" s="8">
         <v>3.5</v>
       </c>
-      <c r="E8" s="8">
-        <f>C8 * D8</f>
-        <v>7</v>
-      </c>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="13">
@@ -913,56 +930,77 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E11" s="9">
-        <f>E6+E7+E8+E9</f>
-        <v>101.72</v>
+        <f>SUM(E6:E9)</f>
+        <v>94.72</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="13"/>
+      <c r="D12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12">
+        <f>COUNT(E6:E9)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="13"/>
+      <c r="D13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13">
+        <f>COUNTA(A6:A9)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="13"/>
+      <c r="D14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14">
+        <f>COUNTBLANK(E6:E9)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="13"/>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="1:7">
       <c r="B18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="12">
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="1:7">
       <c r="B20" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
+    </row>
+    <row r="21" spans="1:7">
       <c r="B21" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="8">
         <v>80</v>
@@ -976,17 +1014,17 @@
         <v>72</v>
       </c>
       <c r="F21" s="9">
-        <f>E21+$C$18</f>
+        <f t="shared" ref="F21:G23" si="0">E21+$C$18</f>
         <v>72.099999999999994</v>
       </c>
       <c r="G21" s="9">
-        <f>F21+$C$18</f>
+        <f t="shared" si="0"/>
         <v>72.199999999999989</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="1:7">
       <c r="B22" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="8">
         <v>80</v>
@@ -1000,17 +1038,17 @@
         <v>72</v>
       </c>
       <c r="F22" s="9">
-        <f>E22+$C$18</f>
+        <f t="shared" si="0"/>
         <v>72.099999999999994</v>
       </c>
       <c r="G22" s="9">
-        <f>F22+$C$18</f>
+        <f t="shared" si="0"/>
         <v>72.199999999999989</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="1:7">
       <c r="B23" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="8">
         <v>95</v>
@@ -1024,15 +1062,31 @@
         <v>85.5</v>
       </c>
       <c r="F23" s="9">
-        <f>E23+$C$18</f>
+        <f t="shared" si="0"/>
         <v>85.6</v>
       </c>
       <c r="G23" s="9">
-        <f>F23+$C$18</f>
+        <f t="shared" si="0"/>
         <v>85.699999999999989</v>
       </c>
     </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="1:7">
+      <c r="A30" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>6</v>
+      </c>
+      <c r="E30" s="16">
+        <f>MEDIAN(B30:D30)</f>
+        <v>6</v>
+      </c>
       <c r="F30" s="11"/>
     </row>
   </sheetData>

</xml_diff>